<commit_message>
1. add RF revicer program.
</commit_message>
<xml_diff>
--- a/doc/program.xlsx
+++ b/doc/program.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RF Receiver" sheetId="1" r:id="rId1"/>
+    <sheet name="RF Sender" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -141,6 +142,429 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21E9590A-1AE9-4CF2-8E15-F74B66158B80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1524000" y="542925"/>
+          <a:ext cx="4514850" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Init:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>1. Init</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> GPIO      LED &amp; RF Revicer Pin &amp; RF Sender Pin</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>2. Init Ext Int0  Capture Falling Edge of RF Revicer Pin</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>3. Init Timer     Count the Falling Edge times</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48A84601-F9C4-4669-8FCE-65A8CAE08C18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2419350" y="1905000"/>
+          <a:ext cx="2724150" cy="447675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Wait</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> for Wake_Up Pin Falling Edge</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F2E517C-66DC-4EB9-B4EA-63A58E8C7E0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1847849" y="2952750"/>
+          <a:ext cx="3857625" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Get</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> Falling Eage, then check system_status to Start/Stop</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77ECAC56-7E1F-48B8-94FA-0026D3039F05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="3" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3781425" y="1314450"/>
+          <a:ext cx="0" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>347662</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4AFBCE2-7E4B-416E-AD09-EBF0517BDD14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3776662" y="2352675"/>
+          <a:ext cx="4763" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1426031" cy="257506"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{299E1B91-D00F-46D3-B186-A7B2C39A16AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3752850" y="2505075"/>
+          <a:ext cx="1426031" cy="257506"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>get falling edge</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,9 +832,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>